<commit_message>
The program is improved
</commit_message>
<xml_diff>
--- a/files/Patient.xlsx
+++ b/files/Patient.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21528"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64D79A82-4AA2-4523-A046-EC6D3E1BB8EB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C73B6E1-FB15-46CE-A99A-05128AB6F52F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Фамилия И. О.</t>
   </si>
@@ -34,10 +34,16 @@
     <t>Пол</t>
   </si>
   <si>
+    <t>Диагноз</t>
+  </si>
+  <si>
     <t>Ширяев Д. А.</t>
   </si>
   <si>
     <t>М</t>
+  </si>
+  <si>
+    <t>Обследование</t>
   </si>
 </sst>
 </file>
@@ -389,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -400,7 +406,7 @@
     <col min="1" max="1" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -410,20 +416,22 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="E1">
-        <f>COUNTIF(A1:A10000,"&lt;&gt;")</f>
-        <v>2</v>
+      <c r="D1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>